<commit_message>
Added sprint backlog #2
</commit_message>
<xml_diff>
--- a/ProjectAndSprintBacklog.xlsx
+++ b/ProjectAndSprintBacklog.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Opis" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Product Backlog" sheetId="2" state="visible" r:id="rId4"/>
     <sheet name="Sprint Backlog #1" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Sprint Backlog #2" sheetId="4" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="66">
   <si>
     <t xml:space="preserve">Sorting Madness</t>
   </si>
@@ -212,6 +213,30 @@
   </si>
   <si>
     <t xml:space="preserve">Wprowadzenie rejestru sprintu do narzędzia zarządzania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dopracowanie poprawności i stabilności programu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 * 5 = 20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Brak nowych elementów rejestru, ten sprint skupia się na testowaniu programu i ewentualnych poprawkach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dokładne Testowanie algorytmów </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    więcej testów</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    przypadki brzegowe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    testowanie za pomocą mockito</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Testowanie stabilności aplikacji</t>
   </si>
 </sst>
 </file>
@@ -366,7 +391,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -474,6 +499,17 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela3" displayName="Tabela3" ref="A4:C44" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A4:C44"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Element rejestru produktu"/>
+    <tableColumn id="2" name="Zadania"/>
+    <tableColumn id="3" name="Pracochłonność "/>
+  </tableColumns>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabela3_2" displayName="Tabela3_2" ref="A4:C44" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A4:C44"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Element rejestru produktu"/>
@@ -798,7 +834,7 @@
   </sheetPr>
   <dimension ref="A2:G46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1134,6 +1170,249 @@
         <v>2</v>
       </c>
     </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+  <tableParts>
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A2:G58"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.16796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="45.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="48.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="33"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="E2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+    </row>
+    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="49.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>20</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="6" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="6" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="6" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="9"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="9"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="9"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="9"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="9"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="9"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="9"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="9"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="9"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="9"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="9"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1"/>
+      <c r="B25" s="9"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="9"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="9"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="9"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="9"/>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="9"/>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1"/>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="9"/>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="9"/>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="9"/>
+    </row>
+    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="9"/>
+    </row>
+    <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="9"/>
+    </row>
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="9"/>
+    </row>
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="9"/>
+    </row>
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="9"/>
+    </row>
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="9"/>
+    </row>
+    <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="9"/>
+    </row>
+    <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="9"/>
+    </row>
+    <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="B2:C2"/>

</xml_diff>